<commit_message>
Added bible verse for March 11 2020
</commit_message>
<xml_diff>
--- a/bible_quiz/Questions.xlsx
+++ b/bible_quiz/Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software_Development\PRYWorkspace\git\PYR\bible_quiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C013C59-D9B4-4CDF-BE6F-AEC059FEE228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1850A0FD-39C7-415F-9A48-BE6AAD0CF76E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D97C711-F6EA-4A0B-A91E-D50AE7802199}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Bible Quiz</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Mark 5:41</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499532DA-8F20-46CC-A47E-8013B7210293}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -436,6 +439,14 @@
         <v>43900</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>43901</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Bible quiz question for March 12 2020
</commit_message>
<xml_diff>
--- a/bible_quiz/Questions.xlsx
+++ b/bible_quiz/Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software_Development\PRYWorkspace\git\PYR\bible_quiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1850A0FD-39C7-415F-9A48-BE6AAD0CF76E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0224CB36-1E41-4E81-A389-4D03049EB7D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D97C711-F6EA-4A0B-A91E-D50AE7802199}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Bible Quiz</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Mark 5:41</t>
+  </si>
+  <si>
+    <t>Mark 5:42</t>
   </si>
 </sst>
 </file>
@@ -411,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499532DA-8F20-46CC-A47E-8013B7210293}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,6 +450,14 @@
         <v>43901</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>43902</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>